<commit_message>
FTP update for Cobblemon module
</commit_message>
<xml_diff>
--- a/cobblemon_module/output.xlsx
+++ b/cobblemon_module/output.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t xml:space="preserve">Qui a attrapé le plus de Cobblemons ?</t>
   </si>
@@ -35,246 +35,249 @@
     <t xml:space="preserve">2.</t>
   </si>
   <si>
+    <t xml:space="preserve">Julgane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.</t>
+  </si>
+  <si>
     <t xml:space="preserve">HexakiI</t>
   </si>
   <si>
-    <t xml:space="preserve">3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julgane</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.</t>
   </si>
   <si>
+    <t xml:space="preserve">GotagaTV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fukano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Etoiles</t>
   </si>
   <si>
-    <t xml:space="preserve">5.</t>
+    <t xml:space="preserve">7.</t>
   </si>
   <si>
     <t xml:space="preserve">SakorRos</t>
   </si>
   <si>
-    <t xml:space="preserve">6.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fukano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GotagaTV</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.</t>
   </si>
   <si>
+    <t xml:space="preserve">nemenems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.</t>
+  </si>
+  <si>
     <t xml:space="preserve">AntoineDaniel_</t>
   </si>
   <si>
-    <t xml:space="preserve">9.</t>
+    <t xml:space="preserve">10.</t>
   </si>
   <si>
     <t xml:space="preserve">NakaStream</t>
   </si>
   <si>
-    <t xml:space="preserve">10.</t>
+    <t xml:space="preserve">Dernière update le 15.02.25 à 04:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(prochaine update vers 20h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.</t>
   </si>
   <si>
     <t xml:space="preserve">KennyStream</t>
   </si>
   <si>
-    <t xml:space="preserve">Dernière update le 14.02.25 à 23:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(prochaine update vers 20h)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.</t>
+    <t xml:space="preserve">23.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LadySundae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BagheraJones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoMaN_uS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mynth0s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theorus_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.</t>
   </si>
   <si>
     <t xml:space="preserve">_Linca</t>
   </si>
   <si>
-    <t xml:space="preserve">23.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MoMaN_uS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BagheraJones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.</t>
+    <t xml:space="preserve">25.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grimkujow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elspawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChloeRamdani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aypierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxouzboub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.</t>
   </si>
   <si>
     <t xml:space="preserve">ZeratoR</t>
   </si>
   <si>
-    <t xml:space="preserve">24.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LadySundae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theorus_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChloeRamdani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aypierre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elspawn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.</t>
+    <t xml:space="preserve">27.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TheGuill84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nisqylegoat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JimmyBoyyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terraciid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KyriaaTV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.</t>
   </si>
   <si>
     <t xml:space="preserve">Gom4rt_</t>
   </si>
   <si>
-    <t xml:space="preserve">26.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TheGuill84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nisqylegoat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.</t>
+    <t xml:space="preserve">29.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrocodyleTV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HarryLafranc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angle_Droit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mickaplow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wingobear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bebesukita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepito_kawazakii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horty_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onutrem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.</t>
   </si>
   <si>
     <t xml:space="preserve">Brybry_</t>
   </si>
   <si>
-    <t xml:space="preserve">27.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terraciid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxouzboub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angle_Droit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrocodyleTV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HarryLafranc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JimmyBoyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebesukita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wingobear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horty_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mickaplow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mynth0s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pepito_kawazakii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.</t>
+    <t xml:space="preserve">22.</t>
   </si>
   <si>
     <t xml:space="preserve">Bytell2</t>
   </si>
   <si>
-    <t xml:space="preserve">32.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onutrem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nemenems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grimkujow</t>
-  </si>
-  <si>
     <t xml:space="preserve">33.</t>
   </si>
   <si>
@@ -284,7 +287,7 @@
     <t xml:space="preserve">44.</t>
   </si>
   <si>
-    <t xml:space="preserve">(prochaine update vers 01h)</t>
+    <t xml:space="preserve">(prochaine update vers 15:00)</t>
   </si>
 </sst>
 </file>
@@ -438,28 +441,28 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left style="hair"/>
       <right/>
-      <top style="thin"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left style="hair"/>
       <right/>
       <top/>
       <bottom/>
@@ -467,30 +470,30 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
+      <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left style="hair"/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
+      <right style="hair"/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -519,7 +522,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -576,6 +579,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,14 +611,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,23 +643,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -731,7 +742,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.18"/>
@@ -763,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>415</v>
+        <v>462</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -776,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>377</v>
+        <v>421</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -789,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>356</v>
+        <v>415</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -802,7 +813,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>336</v>
+        <v>407</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -815,7 +826,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -828,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>273</v>
+        <v>362</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -841,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>264</v>
+        <v>361</v>
       </c>
       <c r="E9" s="2"/>
       <c r="H9" s="8"/>
@@ -855,7 +866,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -868,7 +879,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -881,7 +892,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="7" t="n">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -934,10 +945,10 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.36"/>
@@ -996,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>415</v>
+        <v>462</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>23</v>
@@ -1004,17 +1015,17 @@
       <c r="F3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="16" t="n">
-        <v>172</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="15" t="n">
+        <v>196</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="16" t="n">
-        <v>96</v>
+      <c r="J3" s="18" t="n">
+        <v>110</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>27</v>
@@ -1022,394 +1033,398 @@
       <c r="L3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="16" t="n">
+      <c r="M3" s="15" t="n">
         <v>38</v>
       </c>
       <c r="N3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="n">
-        <v>377</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="21" t="n">
+        <v>421</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="22" t="n">
-        <v>161</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="G4" s="23" t="n">
+        <v>183</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="22" t="n">
-        <v>96</v>
-      </c>
-      <c r="K4" s="20" t="s">
+      <c r="J4" s="25" t="n">
+        <v>108</v>
+      </c>
+      <c r="K4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="22" t="n">
+      <c r="M4" s="23" t="n">
         <v>28</v>
       </c>
       <c r="N4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="25" t="n">
-        <v>356</v>
-      </c>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="28" t="n">
+        <v>415</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="28" t="n">
-        <v>151</v>
-      </c>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="15" t="n">
+        <v>182</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="28" t="n">
-        <v>83</v>
-      </c>
-      <c r="K5" s="26" t="s">
+      <c r="J5" s="30" t="n">
+        <v>102</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="28" t="n">
+      <c r="M5" s="15" t="n">
         <v>24</v>
       </c>
       <c r="N5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22" t="n">
-        <v>336</v>
-      </c>
-      <c r="E6" s="20" t="s">
+      <c r="D6" s="25" t="n">
+        <v>407</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="22" t="n">
-        <v>145</v>
-      </c>
-      <c r="H6" s="20" t="s">
+      <c r="G6" s="23" t="n">
+        <v>173</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="22" t="n">
-        <v>80</v>
-      </c>
-      <c r="K6" s="20" t="s">
+      <c r="J6" s="25" t="n">
+        <v>100</v>
+      </c>
+      <c r="K6" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="22" t="n">
+      <c r="M6" s="23" t="n">
         <v>19</v>
       </c>
       <c r="N6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="28" t="n">
-        <v>326</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="30" t="n">
+        <v>368</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="28" t="n">
-        <v>141</v>
-      </c>
-      <c r="H7" s="26" t="s">
+      <c r="G7" s="15" t="n">
+        <v>161</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="28" t="n">
-        <v>77</v>
-      </c>
-      <c r="K7" s="26" t="s">
+      <c r="J7" s="30" t="n">
+        <v>80</v>
+      </c>
+      <c r="K7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="28" t="n">
+      <c r="M7" s="15" t="n">
         <v>19</v>
       </c>
       <c r="N7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="22" t="n">
-        <v>273</v>
-      </c>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="25" t="n">
+        <v>362</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="22" t="n">
-        <v>119</v>
-      </c>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="23" t="n">
+        <v>151</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="22" t="n">
-        <v>75</v>
-      </c>
-      <c r="K8" s="20" t="s">
+      <c r="J8" s="25" t="n">
+        <v>77</v>
+      </c>
+      <c r="K8" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="22" t="n">
-        <v>5</v>
+      <c r="M8" s="23" t="n">
+        <v>14</v>
       </c>
       <c r="N8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="28" t="n">
-        <v>264</v>
-      </c>
-      <c r="E9" s="26" t="s">
+      <c r="D9" s="30" t="n">
+        <v>361</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="28" t="n">
-        <v>116</v>
-      </c>
-      <c r="H9" s="26" t="s">
+      <c r="G9" s="15" t="n">
+        <v>145</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="28" t="n">
-        <v>65</v>
-      </c>
-      <c r="K9" s="26" t="s">
+      <c r="J9" s="30" t="n">
+        <v>75</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="28" t="n">
-        <v>0</v>
+      <c r="M9" s="15" t="n">
+        <v>5</v>
       </c>
       <c r="N9" s="2"/>
       <c r="Q9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="22" t="n">
-        <v>240</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="D10" s="25" t="n">
+        <v>271</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="22" t="n">
-        <v>115</v>
-      </c>
-      <c r="H10" s="20" t="s">
+      <c r="G10" s="23" t="n">
+        <v>131</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="22" t="n">
+      <c r="J10" s="25" t="n">
         <v>56</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="21"/>
-      <c r="M10" s="22"/>
+      <c r="L10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="23" t="n">
+        <v>0</v>
+      </c>
       <c r="N10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="28" t="n">
-        <v>214</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="27" t="s">
+      <c r="D11" s="30" t="n">
+        <v>251</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="28" t="n">
-        <v>108</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="F11" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="G11" s="15" t="n">
+        <v>127</v>
+      </c>
+      <c r="H11" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="28" t="n">
+      <c r="I11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="K11" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
+      <c r="K11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="31" t="n">
-        <v>196</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="30" t="s">
+      <c r="D12" s="25" t="n">
+        <v>215</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="31" t="n">
-        <v>107</v>
-      </c>
-      <c r="H12" s="29" t="s">
+      <c r="F12" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="G12" s="23" t="n">
+        <v>115</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="31" t="n">
+      <c r="I12" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="25" t="n">
         <v>49</v>
       </c>
-      <c r="K12" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="30"/>
-      <c r="M12" s="31"/>
+      <c r="K12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
-      <c r="B13" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="27" t="s">
+      <c r="B13" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="28" t="n">
-        <v>177</v>
-      </c>
-      <c r="E13" s="26" t="s">
+      <c r="C13" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="D13" s="33" t="n">
+        <v>202</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="28" t="n">
-        <v>102</v>
-      </c>
-      <c r="H13" s="26" t="s">
+      <c r="F13" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="G13" s="15" t="n">
+        <v>115</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="28" t="n">
+      <c r="I13" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" s="33" t="n">
         <v>39</v>
       </c>
-      <c r="K13" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
+      <c r="K13" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1433,7 +1448,7 @@
     <row r="15" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>

</xml_diff>

<commit_message>
Added option to ignore some names in Cobblemon leaderboard
</commit_message>
<xml_diff>
--- a/cobblemon_module/output.xlsx
+++ b/cobblemon_module/output.xlsx
@@ -53,21 +53,21 @@
     <t xml:space="preserve">5.</t>
   </si>
   <si>
+    <t xml:space="preserve">SakorRos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fukano</t>
   </si>
   <si>
-    <t xml:space="preserve">6.</t>
+    <t xml:space="preserve">7.</t>
   </si>
   <si>
     <t xml:space="preserve">Etoiles</t>
   </si>
   <si>
-    <t xml:space="preserve">7.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SakorRos</t>
-  </si>
-  <si>
     <t xml:space="preserve">8.</t>
   </si>
   <si>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">NakaStream</t>
   </si>
   <si>
-    <t xml:space="preserve">Dernière update le 15.02.25 à 04:14</t>
+    <t xml:space="preserve">Dernière update le 15.02.25 à 04:47</t>
   </si>
   <si>
     <t xml:space="preserve">(prochaine update vers 20h)</t>
@@ -742,7 +742,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.18"/>
@@ -787,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -813,7 +813,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -826,7 +826,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -839,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -852,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E9" s="2"/>
       <c r="H9" s="8"/>
@@ -945,10 +945,10 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.36"/>
@@ -1047,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="21" t="n">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>29</v>
@@ -1056,7 +1056,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="23" t="n">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>31</v>
@@ -1127,7 +1127,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="25" t="n">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>41</v>
@@ -1167,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="30" t="n">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>47</v>
@@ -1207,7 +1207,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="25" t="n">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>53</v>
@@ -1247,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="30" t="n">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
New Shiny Leaderboard feature
</commit_message>
<xml_diff>
--- a/cobblemon_module/output.xlsx
+++ b/cobblemon_module/output.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="leaderboard2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="leaderboard3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,10 +23,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Qui a attrapé le plus de Cobblemons ?</t>
+    <t xml:space="preserve">Qui a attrapé le plus de Cobblemons ?</t>
   </si>
   <si>
-    <t xml:space="preserve">Last updated 16.02.25 at 17:01</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="28"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Source Code Pro Semibold"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Qui a attrapé le plus de </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="28"/>
+        <color rgb="FF00FFFF"/>
+        <rFont val="Source Code Pro Semibold"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Shiny</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="28"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Source Code Pro Semibold"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Cobblemons ?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -35,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -104,8 +137,16 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="28"/>
+      <color rgb="FF00FFFF"/>
+      <name val="Source Code Pro Semibold"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,7 +174,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF003B76"/>
-        <bgColor rgb="FF00274E"/>
+        <bgColor rgb="FF004F9E"/>
       </patternFill>
     </fill>
     <fill>
@@ -152,6 +193,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7B3D00"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008400"/>
+        <bgColor rgb="FF3B7600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF132600"/>
+        <bgColor rgb="FF00274E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF274E00"/>
+        <bgColor rgb="FF3B7600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B7600"/>
+        <bgColor rgb="FF274E00"/>
       </patternFill>
     </fill>
   </fills>
@@ -224,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,6 +395,66 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,9 +478,9 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF008400"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF3B7600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -394,12 +519,12 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003B76"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF00274E"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF132600"/>
+      <rgbColor rgb="FF274E00"/>
       <rgbColor rgb="FF7B3D00"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF004F9E"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF00274E"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -412,11 +537,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
@@ -631,9 +756,7 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
-      <c r="B13" s="25" t="s">
-        <v>1</v>
-      </c>
+      <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -679,8 +802,298 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B14:M14"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="5.28"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+    </row>
+    <row r="2" customFormat="false" ht="83.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="27"/>
+    </row>
+    <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="27"/>
+    </row>
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="27"/>
+    </row>
+    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="27"/>
+    </row>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="27"/>
+    </row>
+    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="27"/>
+    </row>
+    <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="27"/>
+      <c r="Q9" s="24"/>
+    </row>
+    <row r="10" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="27"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="27"/>
+    </row>
+    <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="27"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="27"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="27"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="27"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:M2"/>

</xml_diff>

<commit_message>
Fix LastUpdated in cobblemon config
</commit_message>
<xml_diff>
--- a/cobblemon_module/output.xlsx
+++ b/cobblemon_module/output.xlsx
@@ -1664,7 +1664,7 @@
       <c r="A13" s="71" t="n"/>
       <c r="B13" s="93" t="inlineStr">
         <is>
-          <t>Dernière update le 23.02.25 à 20:34</t>
+          <t>Dernière update le 23.02.25 à 23:23</t>
         </is>
       </c>
       <c r="N13" s="71" t="n"/>
@@ -2325,7 +2325,7 @@
       <c r="A13" s="95" t="n"/>
       <c r="B13" s="113" t="inlineStr">
         <is>
-          <t>Dernière update le 23.02.25 à 20:34</t>
+          <t>Dernière update le 23.02.25 à 23:23</t>
         </is>
       </c>
       <c r="N13" s="95" t="n"/>

</xml_diff>